<commit_message>
Added more steps to system level tests
</commit_message>
<xml_diff>
--- a/SystemLevelTests_MasonRoller.xlsx
+++ b/SystemLevelTests_MasonRoller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason\Documents\NetBeansProjects\Diagrams_CIT_360\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9C45BB-88CB-4E8E-A6EC-6E89B204D502}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D043630-6AC7-4B7C-9419-8EACAB2179DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B07AFA53-E78E-4E35-9DE1-0A0E12149CAE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -128,13 +128,112 @@
   </si>
   <si>
     <t>Failed due to no new planogram replacing the old one. Look at step 2</t>
+  </si>
+  <si>
+    <t>Planogram_4</t>
+  </si>
+  <si>
+    <t>Planogram_5</t>
+  </si>
+  <si>
+    <t>Planogram_6</t>
+  </si>
+  <si>
+    <t>Planogram_7</t>
+  </si>
+  <si>
+    <t>Planogram_8</t>
+  </si>
+  <si>
+    <t>Old and new planogram information/pdfs</t>
+  </si>
+  <si>
+    <t>System sends new planogram information sent to the store</t>
+  </si>
+  <si>
+    <t>System sends the new information to the store during nightly process</t>
+  </si>
+  <si>
+    <t>Store employees swap out the planograms in store and marks it done in the system</t>
+  </si>
+  <si>
+    <t>Employee clicks done on an application when finished swapping the planograms</t>
+  </si>
+  <si>
+    <t>Planogram data from old to new in the application</t>
+  </si>
+  <si>
+    <t>System marks that the planograms were swapped</t>
+  </si>
+  <si>
+    <t>System creates a shipping label and internal order to send back old product</t>
+  </si>
+  <si>
+    <t>System creates a cost effective shipping label and internal order to send back old product to the warehouse</t>
+  </si>
+  <si>
+    <t>Old planogram data and how much was in the store when swapped</t>
+  </si>
+  <si>
+    <t>Shipping label and internal order created</t>
+  </si>
+  <si>
+    <t>New information shows up in the store in the morning or shows up in the nightly extract to test</t>
+  </si>
+  <si>
+    <t>Can just look at the extract rather than waiting overnight to see results.</t>
+  </si>
+  <si>
+    <t>Store employees ship back old planograms/products and it gets processed in the warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store employees ships back the planograms/products to the warehouse and then the warehouse processes the items to be stored </t>
+  </si>
+  <si>
+    <t>Old planogram/product data and how much of it there is</t>
+  </si>
+  <si>
+    <t>Items are received in the warehouse and stored</t>
+  </si>
+  <si>
+    <t>Can look at the warehouse item count to ensure that they are there</t>
+  </si>
+  <si>
+    <t>Corporate or the system determines when and if to sell the old products to a third party or back to the vendor</t>
+  </si>
+  <si>
+    <t>Employee or System determines the best time and price/cost to sell the products</t>
+  </si>
+  <si>
+    <t>Price at which product was bought and price at what it can be sold for</t>
+  </si>
+  <si>
+    <t>Sell products/items when the loss ratio is at an acceptable level as set by corporate</t>
+  </si>
+  <si>
+    <t>Loss amount differs by item, to test just make sure it works at the nightly level to catch the best price</t>
+  </si>
+  <si>
+    <t>New information not sent to store</t>
+  </si>
+  <si>
+    <t>Cant swap planograms as there is no new planogram</t>
+  </si>
+  <si>
+    <t>Cant create an order/shipping label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No items expected/received </t>
+  </si>
+  <si>
+    <t>Cant sell items when not in warehouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +245,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -491,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9368B90D-4C60-4A67-AD16-299B2954DC6F}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,11 +607,11 @@
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -590,7 +695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -616,7 +721,147 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -624,10 +869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE858A6B-52E0-4472-801F-3A698DCC400D}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -756,7 +1001,153 @@
         <v>31</v>
       </c>
     </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>